<commit_message>
File with 2 dummy users set to the first step
</commit_message>
<xml_diff>
--- a/Journey/Moms Adopting Moms.xlsx
+++ b/Journey/Moms Adopting Moms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\MomsAdoptingMomsApp\Journey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A75CBD-10DA-406E-BF3D-F2129B570D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28D96B2-54AE-4690-8E9A-EB85ADCFAD03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="1510" windowWidth="14400" windowHeight="8190" xr2:uid="{9DCAD52C-84BE-4AF3-B825-71EFCDBBA0E3}"/>
+    <workbookView xWindow="38772" yWindow="2700" windowWidth="30936" windowHeight="16776" xr2:uid="{9DCAD52C-84BE-4AF3-B825-71EFCDBBA0E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Bio Mom Data" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="52">
   <si>
     <t>Parent ID</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>Peachtree</t>
-  </si>
-  <si>
-    <t>StepA</t>
   </si>
   <si>
     <t>Case Worker 1</t>
@@ -555,48 +552,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3857F66-7078-4FE9-A93C-5704645FD13F}">
   <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AH2" sqref="AH2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.26953125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="15.265625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.53125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.40625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.53125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.53125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.40625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.53125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.3984375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.1328125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.86328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.73046875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.53125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.73046875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.40625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.40625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.3984375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.53125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.265625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="25.86328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.40625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.73046875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="18.86328125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -700,7 +697,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>12345</v>
       </c>
@@ -714,10 +711,10 @@
         <v>48201</v>
       </c>
       <c r="AH2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>67890</v>
       </c>
@@ -731,7 +728,7 @@
         <v>30303</v>
       </c>
       <c r="AH3" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -748,51 +745,51 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="5" width="14.54296875" customWidth="1"/>
-    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="14.53125" customWidth="1"/>
+    <col min="6" max="6" width="10.53125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.40625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.53125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.53125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.53125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="30" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.40625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.3984375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.1328125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7.86328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.73046875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.53125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.73046875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="15.1328125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="25.86328125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.40625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.73046875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="18.86328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -822,52 +819,52 @@
         <v>11</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -883,24 +880,24 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.53125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.40625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.53125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.53125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.53125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.40625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.3984375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="30" width="1.40625" bestFit="1" customWidth="1"/>
+    <col min="17" max="30" width="1.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -929,55 +926,55 @@
         <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -993,24 +990,24 @@
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.53125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.40625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.53125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.53125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.53125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.40625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.3984375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="30" width="1.40625" bestFit="1" customWidth="1"/>
+    <col min="17" max="30" width="1.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1039,49 +1036,49 @@
         <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1097,19 +1094,19 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.53125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.53125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -1118,10 +1115,10 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" t="s">
-        <v>51</v>
       </c>
       <c r="F1" t="s">
         <v>11</v>

</xml_diff>